<commit_message>
EMI filters, ferrite beads
</commit_message>
<xml_diff>
--- a/docs/a500-bom.xlsx
+++ b/docs/a500-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="531">
   <si>
     <t>Part Id</t>
   </si>
@@ -46,7 +46,7 @@
     <t>PCB Assembly (PAL)</t>
   </si>
   <si>
-    <t>Rämixx 500 by SukkoPera</t>
+    <t>Rämixx500 by SukkoPera</t>
   </si>
   <si>
     <t>312812-02</t>
@@ -490,7 +490,7 @@
     <t>900463-16</t>
   </si>
   <si>
-    <t>1000pF - MLC X7R</t>
+    <t>1nF - MLC X7R</t>
   </si>
   <si>
     <t>80-C420C102J1G-TR</t>
@@ -502,7 +502,7 @@
     <t>900463-23</t>
   </si>
   <si>
-    <t>3900pF - MLC X7R</t>
+    <t>3.9nF - MLC X7R</t>
   </si>
   <si>
     <t>80-C430C392GAG5TA</t>
@@ -514,7 +514,7 @@
     <t>900463-26</t>
   </si>
   <si>
-    <t>6800pF - MLC X7R</t>
+    <t>6.8nF - MLC X7R</t>
   </si>
   <si>
     <t>80-C430C682GAG5TA</t>
@@ -964,7 +964,10 @@
     <t>251842-02</t>
   </si>
   <si>
-    <t>EMI Filter 100pF</t>
+    <t>EMI Filter 100pF, no ferrite</t>
+  </si>
+  <si>
+    <t>Murata DSN6NC51H101</t>
   </si>
   <si>
     <t>TH-3</t>
@@ -979,6 +982,12 @@
     <t>EMI Filter 150pF</t>
   </si>
   <si>
+    <t>Murata DSS1NB32A151</t>
+  </si>
+  <si>
+    <t>81-DSS1NB32A151Q91A</t>
+  </si>
+  <si>
     <t>E402 E434 E532 E534</t>
   </si>
   <si>
@@ -988,6 +997,12 @@
     <t>EMI Filter 270pF</t>
   </si>
   <si>
+    <t>Murata DSS1NB32A271</t>
+  </si>
+  <si>
+    <t>81-DSS1NB32A271Q91A</t>
+  </si>
+  <si>
     <t>E305 E306</t>
   </si>
   <si>
@@ -997,13 +1012,25 @@
     <t>EMI Filter 470pF</t>
   </si>
   <si>
+    <t>Murata DSS1NB32A471</t>
+  </si>
+  <si>
+    <t>81-DSS1NB32A471Q91A</t>
+  </si>
+  <si>
     <t>E415 E416 E417 E425 E426 E427 E441 E442 E443 E444 E520 E531 E533 E535 E536 E537 E538</t>
   </si>
   <si>
     <t>390275-01</t>
   </si>
   <si>
-    <t>EMI Filter 6800pF</t>
+    <t>EMI Filter 6.8nF</t>
+  </si>
+  <si>
+    <t>Murata DSS1NB32A682</t>
+  </si>
+  <si>
+    <t>81-DSS1NB32A682Q91A</t>
   </si>
   <si>
     <t>E302 E303 E411 E412 E413 E414 E421 E422 E423 E424</t>
@@ -1012,7 +1039,13 @@
     <t>390297-05</t>
   </si>
   <si>
-    <t>EMI Filter 0.01µF</t>
+    <t>EMI Filter 10nF</t>
+  </si>
+  <si>
+    <t>Murata DSS1NB32A103</t>
+  </si>
+  <si>
+    <t>81-DSS1NB32A103Q91A</t>
   </si>
   <si>
     <t>E101 E110 E401 E403 E404 E405 E406 E407 E408 E601 E602 E702 E703 E704</t>
@@ -1046,6 +1079,9 @@
   </si>
   <si>
     <t>Radial</t>
+  </si>
+  <si>
+    <t>80-B-01-A</t>
   </si>
   <si>
     <t>FB802</t>
@@ -1589,7 +1625,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.1 (2024-02-29)
+      <t xml:space="preserve">Version: 0.2 (2024-03-25)
 </t>
     </r>
     <r>
@@ -3609,155 +3645,191 @@
       <c r="C83" t="s">
         <v>316</v>
       </c>
+      <c r="D83" t="s">
+        <v>317</v>
+      </c>
       <c r="E83" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B84">
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>320</v>
+        <v>321</v>
+      </c>
+      <c r="D84" t="s">
+        <v>322</v>
       </c>
       <c r="E84" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>323</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>323</v>
+        <v>326</v>
+      </c>
+      <c r="D85" t="s">
+        <v>327</v>
       </c>
       <c r="E85" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>328</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B86">
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>326</v>
+        <v>331</v>
+      </c>
+      <c r="D86" t="s">
+        <v>332</v>
       </c>
       <c r="E86" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B87">
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>329</v>
+        <v>336</v>
+      </c>
+      <c r="D87" t="s">
+        <v>337</v>
       </c>
       <c r="E87" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="B88">
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>332</v>
+        <v>341</v>
+      </c>
+      <c r="D88" t="s">
+        <v>342</v>
       </c>
       <c r="E88" t="s">
-        <v>317</v>
+        <v>318</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="D89" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="E89" t="s">
         <v>132</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="E90" t="s">
         <v>132</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="E91" t="s">
-        <v>343</v>
+        <v>354</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3768,61 +3840,61 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="E93" t="s">
         <v>60</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="E94" t="s">
         <v>60</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="E95" t="s">
         <v>132</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3833,285 +3905,285 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="D97" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="E97" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="D98" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="D99" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="D100" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="E100" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="D101" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="E101" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D102" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
       <c r="E102" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="D103" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="D104" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="E104" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="B105">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="D105" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="D106" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="E106" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="D107" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="E107" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="D108" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="E108" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="D109" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="E109" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="2" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4122,38 +4194,38 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="D111" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4164,22 +4236,22 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="B114">
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="D114" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="E114" t="s">
         <v>33</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>34</v>
@@ -4187,22 +4259,22 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="D115" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="E115" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>43</v>
@@ -4210,45 +4282,45 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="D116" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="E116" t="s">
         <v>23</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="D117" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="E117" t="s">
         <v>38</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>39</v>
@@ -4256,22 +4328,22 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="D118" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="E118" t="s">
         <v>17</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>18</v>
@@ -4279,7 +4351,7 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="2" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4293,13 +4365,13 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="E120" t="s">
         <v>110</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>112</v>
@@ -4310,16 +4382,16 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="E121" t="s">
         <v>60</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4327,16 +4399,16 @@
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="E122" t="s">
         <v>65</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4344,13 +4416,13 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="E123" t="s">
         <v>47</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>48</v>
@@ -4358,22 +4430,22 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="B124">
         <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="E124" t="s">
         <v>51</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4387,7 +4459,7 @@
         <v>307</v>
       </c>
       <c r="D125" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="E125" t="s">
         <v>292</v>
@@ -4396,7 +4468,7 @@
         <v>308</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4404,21 +4476,21 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="D126" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="E126" t="s">
         <v>179</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="2" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4432,19 +4504,19 @@
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="D128" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
       <c r="E128" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4452,19 +4524,19 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="D129" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="E129" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4472,19 +4544,19 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="D130" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
       <c r="E130" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4498,7 +4570,7 @@
         <v>130</v>
       </c>
       <c r="D131" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="E131" t="s">
         <v>132</v>
@@ -4507,7 +4579,7 @@
         <v>133</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4521,7 +4593,7 @@
         <v>125</v>
       </c>
       <c r="D132" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="E132" t="s">
         <v>117</v>
@@ -4530,7 +4602,7 @@
         <v>126</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4544,7 +4616,7 @@
         <v>257</v>
       </c>
       <c r="D133" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="E133" t="s">
         <v>132</v>
@@ -4553,7 +4625,7 @@
         <v>258</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4567,7 +4639,7 @@
         <v>261</v>
       </c>
       <c r="D134" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="E134" t="s">
         <v>132</v>
@@ -4576,7 +4648,7 @@
         <v>262</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4590,7 +4662,7 @@
         <v>142</v>
       </c>
       <c r="D135" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="E135" t="s">
         <v>138</v>
@@ -4599,7 +4671,7 @@
         <v>143</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4607,19 +4679,19 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="D136" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="E136" t="s">
         <v>132</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4627,16 +4699,16 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="E137" t="s">
         <v>132</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4644,16 +4716,16 @@
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="D138" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4661,16 +4733,16 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="D139" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4678,18 +4750,18 @@
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="D140" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="60" customHeight="1">
       <c r="A142" s="5" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>
@@ -4771,41 +4843,47 @@
     <hyperlink ref="F79" r:id="rId58"/>
     <hyperlink ref="F80" r:id="rId59"/>
     <hyperlink ref="F81" r:id="rId60"/>
-    <hyperlink ref="F95" r:id="rId61"/>
-    <hyperlink ref="F97" r:id="rId62"/>
-    <hyperlink ref="F98" r:id="rId63"/>
-    <hyperlink ref="F99" r:id="rId64"/>
-    <hyperlink ref="F101" r:id="rId65"/>
-    <hyperlink ref="F102" r:id="rId66"/>
-    <hyperlink ref="F105" r:id="rId67"/>
-    <hyperlink ref="F106" r:id="rId68"/>
-    <hyperlink ref="F107" r:id="rId69"/>
-    <hyperlink ref="F108" r:id="rId70"/>
-    <hyperlink ref="F109" r:id="rId71"/>
-    <hyperlink ref="F114" r:id="rId72"/>
-    <hyperlink ref="F115" r:id="rId73"/>
-    <hyperlink ref="F116" r:id="rId74"/>
-    <hyperlink ref="F117" r:id="rId75"/>
-    <hyperlink ref="F118" r:id="rId76"/>
-    <hyperlink ref="F120" r:id="rId77"/>
-    <hyperlink ref="F121" r:id="rId78"/>
-    <hyperlink ref="F122" r:id="rId79"/>
-    <hyperlink ref="F123" r:id="rId80"/>
-    <hyperlink ref="F124" r:id="rId81"/>
-    <hyperlink ref="F125" r:id="rId82"/>
-    <hyperlink ref="F128" r:id="rId83"/>
-    <hyperlink ref="F129" r:id="rId84"/>
-    <hyperlink ref="F130" r:id="rId85"/>
-    <hyperlink ref="F131" r:id="rId86"/>
-    <hyperlink ref="F132" r:id="rId87"/>
-    <hyperlink ref="F133" r:id="rId88"/>
-    <hyperlink ref="F134" r:id="rId89"/>
-    <hyperlink ref="F135" r:id="rId90"/>
-    <hyperlink ref="F136" r:id="rId91"/>
-    <hyperlink ref="F137" r:id="rId92"/>
-    <hyperlink ref="F138" r:id="rId93"/>
-    <hyperlink ref="F139" r:id="rId94"/>
-    <hyperlink ref="F140" r:id="rId95"/>
+    <hyperlink ref="F84" r:id="rId61"/>
+    <hyperlink ref="F85" r:id="rId62"/>
+    <hyperlink ref="F86" r:id="rId63"/>
+    <hyperlink ref="F87" r:id="rId64"/>
+    <hyperlink ref="F88" r:id="rId65"/>
+    <hyperlink ref="F91" r:id="rId66"/>
+    <hyperlink ref="F95" r:id="rId67"/>
+    <hyperlink ref="F97" r:id="rId68"/>
+    <hyperlink ref="F98" r:id="rId69"/>
+    <hyperlink ref="F99" r:id="rId70"/>
+    <hyperlink ref="F101" r:id="rId71"/>
+    <hyperlink ref="F102" r:id="rId72"/>
+    <hyperlink ref="F105" r:id="rId73"/>
+    <hyperlink ref="F106" r:id="rId74"/>
+    <hyperlink ref="F107" r:id="rId75"/>
+    <hyperlink ref="F108" r:id="rId76"/>
+    <hyperlink ref="F109" r:id="rId77"/>
+    <hyperlink ref="F114" r:id="rId78"/>
+    <hyperlink ref="F115" r:id="rId79"/>
+    <hyperlink ref="F116" r:id="rId80"/>
+    <hyperlink ref="F117" r:id="rId81"/>
+    <hyperlink ref="F118" r:id="rId82"/>
+    <hyperlink ref="F120" r:id="rId83"/>
+    <hyperlink ref="F121" r:id="rId84"/>
+    <hyperlink ref="F122" r:id="rId85"/>
+    <hyperlink ref="F123" r:id="rId86"/>
+    <hyperlink ref="F124" r:id="rId87"/>
+    <hyperlink ref="F125" r:id="rId88"/>
+    <hyperlink ref="F128" r:id="rId89"/>
+    <hyperlink ref="F129" r:id="rId90"/>
+    <hyperlink ref="F130" r:id="rId91"/>
+    <hyperlink ref="F131" r:id="rId92"/>
+    <hyperlink ref="F132" r:id="rId93"/>
+    <hyperlink ref="F133" r:id="rId94"/>
+    <hyperlink ref="F134" r:id="rId95"/>
+    <hyperlink ref="F135" r:id="rId96"/>
+    <hyperlink ref="F136" r:id="rId97"/>
+    <hyperlink ref="F137" r:id="rId98"/>
+    <hyperlink ref="F138" r:id="rId99"/>
+    <hyperlink ref="F139" r:id="rId100"/>
+    <hyperlink ref="F140" r:id="rId101"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Review docs and filters
</commit_message>
<xml_diff>
--- a/docs/a500-bom.xlsx
+++ b/docs/a500-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="536">
   <si>
     <t>Part Id</t>
   </si>
@@ -967,12 +967,15 @@
     <t>EMI Filter 100pF, no ferrite</t>
   </si>
   <si>
-    <t>Murata DSN6NC51H101</t>
+    <t>Murata DSN6NC51H101, replacement is with ferrite</t>
   </si>
   <si>
     <t>TH-3</t>
   </si>
   <si>
+    <t>81-DSS1NB32A101Q91A</t>
+  </si>
+  <si>
     <t>E511 E512 E513 E514 E515 E516 E517 E518 E519 E521 E522 E523 E524 E611 E612 E613 E614 E615 E616 E617 E618 E619 E620 E621 E622 E623 E624 E625 E626 E631 E632</t>
   </si>
   <si>
@@ -1069,6 +1072,9 @@
     <t>Ferrite Bead</t>
   </si>
   <si>
+    <t>542-FB20020-4B-RC</t>
+  </si>
+  <si>
     <t>E431 E432 E433 E435</t>
   </si>
   <si>
@@ -1081,7 +1087,7 @@
     <t>Radial</t>
   </si>
   <si>
-    <t>80-B-01-A</t>
+    <t>434-BEAD-10-600P-02</t>
   </si>
   <si>
     <t>FB802</t>
@@ -1225,7 +1231,7 @@
     <t>5 Pin Square DIN</t>
   </si>
   <si>
-    <t>Power Dynamics DS-215</t>
+    <t>Power Dynamics DS-215. Rämixx500 see below.</t>
   </si>
   <si>
     <t>CN8</t>
@@ -1604,6 +1610,15 @@
   </si>
   <si>
     <t>200-SNT100BKG</t>
+  </si>
+  <si>
+    <t>6 Pin Round DIN</t>
+  </si>
+  <si>
+    <t>CN8 alternative. Requires modification to PSU cable!</t>
+  </si>
+  <si>
+    <t>490-SDF-60J</t>
   </si>
   <si>
     <r>
@@ -2059,7 +2074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3651,185 +3666,191 @@
       <c r="E83" t="s">
         <v>318</v>
       </c>
+      <c r="F83" s="4" t="s">
+        <v>319</v>
+      </c>
       <c r="G83" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B84">
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D84" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E84" t="s">
         <v>318</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D85" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E85" t="s">
         <v>318</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B86">
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D86" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E86" t="s">
         <v>318</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B87">
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D87" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E87" t="s">
         <v>318</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B88">
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D88" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E88" t="s">
         <v>318</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D89" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E89" t="s">
         <v>132</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E90" t="s">
         <v>132</v>
       </c>
+      <c r="F90" s="4" t="s">
+        <v>352</v>
+      </c>
       <c r="G90" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E91" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3840,61 +3861,61 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E93" t="s">
         <v>60</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E94" t="s">
         <v>60</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E95" t="s">
         <v>132</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3905,285 +3926,285 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D97" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E97" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D98" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D99" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D100" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E100" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D101" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E101" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D102" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E102" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D103" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D104" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E104" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B105">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D105" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D106" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="E106" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D107" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="E107" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D108" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E108" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D109" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="E109" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4194,38 +4215,38 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D111" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4236,22 +4257,22 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B114">
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D114" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E114" t="s">
         <v>33</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>34</v>
@@ -4259,22 +4280,22 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D115" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E115" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>43</v>
@@ -4282,45 +4303,45 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D116" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="E116" t="s">
         <v>23</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D117" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E117" t="s">
         <v>38</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>39</v>
@@ -4328,22 +4349,22 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D118" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E118" t="s">
         <v>17</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>18</v>
@@ -4351,7 +4372,7 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4365,13 +4386,13 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E120" t="s">
         <v>110</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>112</v>
@@ -4382,16 +4403,16 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="E121" t="s">
         <v>60</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4399,16 +4420,16 @@
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E122" t="s">
         <v>65</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4416,13 +4437,13 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E123" t="s">
         <v>47</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>48</v>
@@ -4430,22 +4451,22 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B124">
         <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E124" t="s">
         <v>51</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4459,7 +4480,7 @@
         <v>307</v>
       </c>
       <c r="D125" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E125" t="s">
         <v>292</v>
@@ -4468,7 +4489,7 @@
         <v>308</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -4476,21 +4497,21 @@
         <v>1</v>
       </c>
       <c r="C126" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D126" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="E126" t="s">
         <v>179</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4504,19 +4525,19 @@
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D128" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E128" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -4524,19 +4545,19 @@
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D129" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E129" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4544,19 +4565,19 @@
         <v>2</v>
       </c>
       <c r="C130" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D130" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E130" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4570,7 +4591,7 @@
         <v>130</v>
       </c>
       <c r="D131" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E131" t="s">
         <v>132</v>
@@ -4579,7 +4600,7 @@
         <v>133</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4593,7 +4614,7 @@
         <v>125</v>
       </c>
       <c r="D132" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E132" t="s">
         <v>117</v>
@@ -4602,7 +4623,7 @@
         <v>126</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4616,7 +4637,7 @@
         <v>257</v>
       </c>
       <c r="D133" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E133" t="s">
         <v>132</v>
@@ -4625,7 +4646,7 @@
         <v>258</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4639,7 +4660,7 @@
         <v>261</v>
       </c>
       <c r="D134" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E134" t="s">
         <v>132</v>
@@ -4648,7 +4669,7 @@
         <v>262</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4662,7 +4683,7 @@
         <v>142</v>
       </c>
       <c r="D135" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="E135" t="s">
         <v>138</v>
@@ -4671,7 +4692,7 @@
         <v>143</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4679,19 +4700,19 @@
         <v>1</v>
       </c>
       <c r="C136" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="D136" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="E136" t="s">
         <v>132</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4699,16 +4720,16 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E137" t="s">
         <v>132</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4716,16 +4737,16 @@
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D138" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4733,16 +4754,16 @@
         <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D139" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4750,18 +4771,35 @@
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D140" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="60" customHeight="1">
-      <c r="A142" s="5" t="s">
-        <v>530</v>
+        <v>531</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="B141">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>532</v>
+      </c>
+      <c r="D141" t="s">
+        <v>533</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="60" customHeight="1">
+      <c r="A143" s="5" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -4780,7 +4818,7 @@
     <mergeCell ref="A113:G113"/>
     <mergeCell ref="A119:G119"/>
     <mergeCell ref="A127:G127"/>
-    <mergeCell ref="A142:G142"/>
+    <mergeCell ref="A143:G143"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F16" r:id="rId1"/>
@@ -4843,47 +4881,50 @@
     <hyperlink ref="F79" r:id="rId58"/>
     <hyperlink ref="F80" r:id="rId59"/>
     <hyperlink ref="F81" r:id="rId60"/>
-    <hyperlink ref="F84" r:id="rId61"/>
-    <hyperlink ref="F85" r:id="rId62"/>
-    <hyperlink ref="F86" r:id="rId63"/>
-    <hyperlink ref="F87" r:id="rId64"/>
-    <hyperlink ref="F88" r:id="rId65"/>
-    <hyperlink ref="F91" r:id="rId66"/>
-    <hyperlink ref="F95" r:id="rId67"/>
-    <hyperlink ref="F97" r:id="rId68"/>
-    <hyperlink ref="F98" r:id="rId69"/>
-    <hyperlink ref="F99" r:id="rId70"/>
-    <hyperlink ref="F101" r:id="rId71"/>
-    <hyperlink ref="F102" r:id="rId72"/>
-    <hyperlink ref="F105" r:id="rId73"/>
-    <hyperlink ref="F106" r:id="rId74"/>
-    <hyperlink ref="F107" r:id="rId75"/>
-    <hyperlink ref="F108" r:id="rId76"/>
-    <hyperlink ref="F109" r:id="rId77"/>
-    <hyperlink ref="F114" r:id="rId78"/>
-    <hyperlink ref="F115" r:id="rId79"/>
-    <hyperlink ref="F116" r:id="rId80"/>
-    <hyperlink ref="F117" r:id="rId81"/>
-    <hyperlink ref="F118" r:id="rId82"/>
-    <hyperlink ref="F120" r:id="rId83"/>
-    <hyperlink ref="F121" r:id="rId84"/>
-    <hyperlink ref="F122" r:id="rId85"/>
-    <hyperlink ref="F123" r:id="rId86"/>
-    <hyperlink ref="F124" r:id="rId87"/>
-    <hyperlink ref="F125" r:id="rId88"/>
-    <hyperlink ref="F128" r:id="rId89"/>
-    <hyperlink ref="F129" r:id="rId90"/>
-    <hyperlink ref="F130" r:id="rId91"/>
-    <hyperlink ref="F131" r:id="rId92"/>
-    <hyperlink ref="F132" r:id="rId93"/>
-    <hyperlink ref="F133" r:id="rId94"/>
-    <hyperlink ref="F134" r:id="rId95"/>
-    <hyperlink ref="F135" r:id="rId96"/>
-    <hyperlink ref="F136" r:id="rId97"/>
-    <hyperlink ref="F137" r:id="rId98"/>
-    <hyperlink ref="F138" r:id="rId99"/>
-    <hyperlink ref="F139" r:id="rId100"/>
-    <hyperlink ref="F140" r:id="rId101"/>
+    <hyperlink ref="F83" r:id="rId61"/>
+    <hyperlink ref="F84" r:id="rId62"/>
+    <hyperlink ref="F85" r:id="rId63"/>
+    <hyperlink ref="F86" r:id="rId64"/>
+    <hyperlink ref="F87" r:id="rId65"/>
+    <hyperlink ref="F88" r:id="rId66"/>
+    <hyperlink ref="F90" r:id="rId67"/>
+    <hyperlink ref="F91" r:id="rId68"/>
+    <hyperlink ref="F95" r:id="rId69"/>
+    <hyperlink ref="F97" r:id="rId70"/>
+    <hyperlink ref="F98" r:id="rId71"/>
+    <hyperlink ref="F99" r:id="rId72"/>
+    <hyperlink ref="F101" r:id="rId73"/>
+    <hyperlink ref="F102" r:id="rId74"/>
+    <hyperlink ref="F105" r:id="rId75"/>
+    <hyperlink ref="F106" r:id="rId76"/>
+    <hyperlink ref="F107" r:id="rId77"/>
+    <hyperlink ref="F108" r:id="rId78"/>
+    <hyperlink ref="F109" r:id="rId79"/>
+    <hyperlink ref="F114" r:id="rId80"/>
+    <hyperlink ref="F115" r:id="rId81"/>
+    <hyperlink ref="F116" r:id="rId82"/>
+    <hyperlink ref="F117" r:id="rId83"/>
+    <hyperlink ref="F118" r:id="rId84"/>
+    <hyperlink ref="F120" r:id="rId85"/>
+    <hyperlink ref="F121" r:id="rId86"/>
+    <hyperlink ref="F122" r:id="rId87"/>
+    <hyperlink ref="F123" r:id="rId88"/>
+    <hyperlink ref="F124" r:id="rId89"/>
+    <hyperlink ref="F125" r:id="rId90"/>
+    <hyperlink ref="F128" r:id="rId91"/>
+    <hyperlink ref="F129" r:id="rId92"/>
+    <hyperlink ref="F130" r:id="rId93"/>
+    <hyperlink ref="F131" r:id="rId94"/>
+    <hyperlink ref="F132" r:id="rId95"/>
+    <hyperlink ref="F133" r:id="rId96"/>
+    <hyperlink ref="F134" r:id="rId97"/>
+    <hyperlink ref="F135" r:id="rId98"/>
+    <hyperlink ref="F136" r:id="rId99"/>
+    <hyperlink ref="F137" r:id="rId100"/>
+    <hyperlink ref="F138" r:id="rId101"/>
+    <hyperlink ref="F139" r:id="rId102"/>
+    <hyperlink ref="F140" r:id="rId103"/>
+    <hyperlink ref="F141" r:id="rId104"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ULP sockets for the DRAMs
</commit_message>
<xml_diff>
--- a/docs/a500-bom.xlsx
+++ b/docs/a500-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="541">
   <si>
     <t>Part Id</t>
   </si>
@@ -1483,7 +1483,13 @@
     <t>575-11044320</t>
   </si>
   <si>
-    <t>U10 U11 U12 U13 U16 U17 U18 U19 U20 U21 U22 U23 U34 U35 U40 U41</t>
+    <t>U10 U11 U12 U13 U34 U35 U40 U41</t>
+  </si>
+  <si>
+    <t>Socket, DIP20, Ultra Low Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 575-115433203</t>
   </si>
   <si>
     <t>Optional bus termination, not populated on original boards</t>
@@ -1649,7 +1655,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.3 (2024-03-25)
+      <t xml:space="preserve">Version: 0.4 (2024-04-07)
 </t>
     </r>
     <r>
@@ -2083,7 +2089,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4499,7 +4505,7 @@
         <v>486</v>
       </c>
       <c r="B124">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
         <v>487</v>
@@ -4516,133 +4522,130 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
+        <v>486</v>
+      </c>
+      <c r="B125">
+        <v>8</v>
+      </c>
+      <c r="C125" t="s">
+        <v>490</v>
+      </c>
+      <c r="E125" t="s">
+        <v>52</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
         <v>307</v>
       </c>
-      <c r="B125">
+      <c r="B126">
         <v>7</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>308</v>
       </c>
-      <c r="D125" t="s">
-        <v>490</v>
-      </c>
-      <c r="E125" t="s">
+      <c r="D126" t="s">
+        <v>492</v>
+      </c>
+      <c r="E126" t="s">
         <v>293</v>
       </c>
-      <c r="F125" s="4" t="s">
+      <c r="F126" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="G125" s="3" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="B126">
-        <v>1</v>
-      </c>
-      <c r="C126" t="s">
-        <v>492</v>
-      </c>
-      <c r="D126" t="s">
+      <c r="G126" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="E126" t="s">
+    </row>
+    <row r="127" spans="1:7">
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>494</v>
+      </c>
+      <c r="D127" t="s">
+        <v>495</v>
+      </c>
+      <c r="E127" t="s">
         <v>180</v>
       </c>
-      <c r="G126" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
+      <c r="G127" s="3" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="128" spans="1:7">
-      <c r="B128">
-        <v>4</v>
-      </c>
-      <c r="C128" t="s">
-        <v>496</v>
-      </c>
-      <c r="D128" t="s">
+      <c r="A128" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="E128" t="s">
-        <v>498</v>
-      </c>
-      <c r="F128" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>500</v>
-      </c>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7">
       <c r="B129">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C129" t="s">
+        <v>498</v>
+      </c>
+      <c r="D129" t="s">
+        <v>499</v>
+      </c>
+      <c r="E129" t="s">
+        <v>500</v>
+      </c>
+      <c r="F129" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="D129" t="s">
+      <c r="G129" s="3" t="s">
         <v>502</v>
-      </c>
-      <c r="E129" t="s">
-        <v>503</v>
-      </c>
-      <c r="F129" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>503</v>
+      </c>
+      <c r="D130" t="s">
+        <v>504</v>
+      </c>
+      <c r="E130" t="s">
+        <v>505</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="B131">
         <v>2</v>
       </c>
-      <c r="C130" t="s">
-        <v>506</v>
-      </c>
-      <c r="D130" t="s">
-        <v>507</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="C131" t="s">
         <v>508</v>
       </c>
-      <c r="F130" s="4" t="s">
+      <c r="D131" t="s">
         <v>509</v>
       </c>
-      <c r="G130" s="3" t="s">
+      <c r="E131" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" t="s">
-        <v>130</v>
-      </c>
-      <c r="B131">
-        <v>1</v>
-      </c>
-      <c r="C131" t="s">
-        <v>131</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="F131" s="4" t="s">
         <v>511</v>
-      </c>
-      <c r="E131" t="s">
-        <v>133</v>
-      </c>
-      <c r="F131" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>512</v>
@@ -4650,22 +4653,22 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D132" t="s">
         <v>513</v>
       </c>
       <c r="E132" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="F132" s="4" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>514</v>
@@ -4673,91 +4676,94 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>257</v>
+        <v>125</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133" t="s">
-        <v>258</v>
+        <v>126</v>
       </c>
       <c r="D133" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E133" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>259</v>
+        <v>127</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B134">
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D134" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E134" t="s">
         <v>133</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>142</v>
+        <v>261</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135" t="s">
-        <v>143</v>
+        <v>262</v>
       </c>
       <c r="D135" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E135" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F135" s="4" t="s">
-        <v>144</v>
+        <v>263</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="136" spans="1:7">
+      <c r="A136" t="s">
+        <v>142</v>
+      </c>
       <c r="B136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136" t="s">
+        <v>143</v>
+      </c>
+      <c r="D136" t="s">
         <v>519</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" t="s">
+        <v>139</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G136" s="3" t="s">
         <v>520</v>
-      </c>
-      <c r="E136" t="s">
-        <v>133</v>
-      </c>
-      <c r="F136" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4765,86 +4771,106 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>523</v>
+        <v>521</v>
+      </c>
+      <c r="D137" t="s">
+        <v>522</v>
       </c>
       <c r="E137" t="s">
         <v>133</v>
       </c>
       <c r="F137" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="G137" s="3" t="s">
         <v>524</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="138" spans="1:7">
       <c r="B138">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C138" t="s">
         <v>525</v>
       </c>
-      <c r="D138" t="s">
-        <v>502</v>
+      <c r="E138" t="s">
+        <v>133</v>
       </c>
       <c r="F138" s="4" t="s">
         <v>526</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>527</v>
+        <v>448</v>
       </c>
     </row>
     <row r="139" spans="1:7">
       <c r="B139">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
+        <v>527</v>
+      </c>
+      <c r="D139" t="s">
+        <v>504</v>
+      </c>
+      <c r="F139" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="D139" t="s">
+      <c r="G139" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="F139" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="G139" s="3" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="140" spans="1:7">
       <c r="B140">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C140" t="s">
+        <v>530</v>
+      </c>
+      <c r="D140" t="s">
+        <v>531</v>
+      </c>
+      <c r="F140" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="D140" t="s">
+      <c r="G140" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="F140" s="4" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="141" spans="1:7">
       <c r="B141">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
+        <v>534</v>
+      </c>
+      <c r="D141" t="s">
         <v>535</v>
       </c>
-      <c r="D141" t="s">
+      <c r="F141" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="F141" s="4" t="s">
+    </row>
+    <row r="142" spans="1:7">
+      <c r="B142">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
         <v>537</v>
       </c>
-      <c r="G141" s="3" t="s">
+      <c r="D142" t="s">
+        <v>538</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G142" s="3" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="60" customHeight="1">
-      <c r="A143" s="5" t="s">
-        <v>538</v>
+    <row r="144" spans="1:7" ht="60" customHeight="1">
+      <c r="A144" s="5" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -4862,8 +4888,8 @@
     <mergeCell ref="A110:G110"/>
     <mergeCell ref="A113:G113"/>
     <mergeCell ref="A119:G119"/>
-    <mergeCell ref="A127:G127"/>
-    <mergeCell ref="A143:G143"/>
+    <mergeCell ref="A128:G128"/>
+    <mergeCell ref="A144:G144"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F16" r:id="rId1"/>
@@ -4956,7 +4982,7 @@
     <hyperlink ref="F123" r:id="rId88"/>
     <hyperlink ref="F124" r:id="rId89"/>
     <hyperlink ref="F125" r:id="rId90"/>
-    <hyperlink ref="F128" r:id="rId91"/>
+    <hyperlink ref="F126" r:id="rId91"/>
     <hyperlink ref="F129" r:id="rId92"/>
     <hyperlink ref="F130" r:id="rId93"/>
     <hyperlink ref="F131" r:id="rId94"/>
@@ -4970,6 +4996,7 @@
     <hyperlink ref="F139" r:id="rId102"/>
     <hyperlink ref="F140" r:id="rId103"/>
     <hyperlink ref="F141" r:id="rId104"/>
+    <hyperlink ref="F142" r:id="rId105"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
No part number for ULP sockets
</commit_message>
<xml_diff>
--- a/docs/a500-bom.xlsx
+++ b/docs/a500-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="541">
   <si>
     <t>Part Id</t>
   </si>
@@ -4521,9 +4521,6 @@
       </c>
     </row>
     <row r="125" spans="1:7">
-      <c r="A125" t="s">
-        <v>486</v>
-      </c>
       <c r="B125">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Fix 74HCT245 part ID (#1)
</commit_message>
<xml_diff>
--- a/docs/a500-bom.xlsx
+++ b/docs/a500-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="546">
   <si>
     <t>Part Id</t>
   </si>
@@ -331,580 +331,583 @@
     <t>U39</t>
   </si>
   <si>
+    <t>380227-06</t>
+  </si>
+  <si>
+    <t>74HCT245, Octal Tri-State Bus Transceiver</t>
+  </si>
+  <si>
+    <t>595-SN74HCT245N</t>
+  </si>
+  <si>
+    <t>U40 U41</t>
+  </si>
+  <si>
+    <t>901523-01</t>
+  </si>
+  <si>
+    <t>NE555, Timer</t>
+  </si>
+  <si>
+    <t>DIP8</t>
+  </si>
+  <si>
+    <t>595-NE555P</t>
+  </si>
+  <si>
+    <t>U42</t>
+  </si>
+  <si>
+    <t>Transistors</t>
+  </si>
+  <si>
+    <t>390254-01</t>
+  </si>
+  <si>
+    <t>MPF102 - N-Channel JFET</t>
+  </si>
+  <si>
+    <t>or PN4302. Rämixx500 SMD alternative: see below</t>
+  </si>
+  <si>
+    <t>TO-92</t>
+  </si>
+  <si>
+    <t>863-MPF102</t>
+  </si>
+  <si>
+    <t>Q321 Q331</t>
+  </si>
+  <si>
+    <t>902658-01</t>
+  </si>
+  <si>
+    <t>2N3904 - NPN</t>
+  </si>
+  <si>
+    <t>637-2N3904</t>
+  </si>
+  <si>
+    <t>Q501 Q711</t>
+  </si>
+  <si>
+    <t>902707-01</t>
+  </si>
+  <si>
+    <t>2N3906 - PNP</t>
+  </si>
+  <si>
+    <t>637-2N3906</t>
+  </si>
+  <si>
+    <t>Q301 Q502 Q503</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>900850-01</t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>or 1N914</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>512-1N4148</t>
+  </si>
+  <si>
+    <t>D501 D911 D912</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>390082-01</t>
+  </si>
+  <si>
+    <t>10nF - MLC Z5U</t>
+  </si>
+  <si>
+    <t>Axial</t>
+  </si>
+  <si>
+    <t>80-C410C103M5R-TR</t>
+  </si>
+  <si>
+    <t>C7 C8 C10 C12 C15 C32 C33 C34 C35 C36 C37 C39 C308 C701 C713 C800 C801 C802 C803</t>
+  </si>
+  <si>
+    <t>390082-02</t>
+  </si>
+  <si>
+    <t>100nF - MLC Z5U</t>
+  </si>
+  <si>
+    <t>80-C412C104K5R-TR</t>
+  </si>
+  <si>
+    <t>C711</t>
+  </si>
+  <si>
+    <t>390082-04</t>
+  </si>
+  <si>
+    <t>330nF - MLC Z5U</t>
+  </si>
+  <si>
+    <t>80-C440C334K5R-TR</t>
+  </si>
+  <si>
+    <t>C1 C2 C3 C4 C5 C6 C9 C11 C13 C14 C16 C17 C18 C19 C20 C40 C41 C42 C301 C302 C305 C325 C335 C501 C502 C804</t>
+  </si>
+  <si>
+    <t>900462-21</t>
+  </si>
+  <si>
+    <t>22pF - MLC NP0</t>
+  </si>
+  <si>
+    <t>594-A220J15C0GH5TAA</t>
+  </si>
+  <si>
+    <t>C911 E666</t>
+  </si>
+  <si>
+    <t>900462-29</t>
+  </si>
+  <si>
+    <t>47pF - MLC NP0</t>
+  </si>
+  <si>
+    <t>594-A470J15C0GH5TAA</t>
+  </si>
+  <si>
+    <t>E102 E103 E106 E107 E108 E109 E791 E792 E793 E794</t>
+  </si>
+  <si>
+    <t>900463-16</t>
+  </si>
+  <si>
+    <t>1nF - MLC X7R</t>
+  </si>
+  <si>
+    <t>80-C420C102J1G-TR</t>
+  </si>
+  <si>
+    <t>C411 C412 C413 C421 C422 C423</t>
+  </si>
+  <si>
+    <t>900463-23</t>
+  </si>
+  <si>
+    <t>3.9nF - MLC X7R</t>
+  </si>
+  <si>
+    <t>80-C430C392GAG5TA</t>
+  </si>
+  <si>
+    <t>C323 C333</t>
+  </si>
+  <si>
+    <t>900463-26</t>
+  </si>
+  <si>
+    <t>6.8nF - MLC X7R</t>
+  </si>
+  <si>
+    <t>80-C430C682GAG5TA</t>
+  </si>
+  <si>
+    <t>C322 C332</t>
+  </si>
+  <si>
+    <t>900463-36</t>
+  </si>
+  <si>
+    <t>47nF - MLC X7R</t>
+  </si>
+  <si>
+    <t>80-C420C473J5G5TA</t>
+  </si>
+  <si>
+    <t>C311 C312 C313 C314</t>
+  </si>
+  <si>
+    <t>900463-37</t>
+  </si>
+  <si>
+    <t>0.1µF - MLC XR7</t>
+  </si>
+  <si>
+    <t>80-C430C104F3G5TA</t>
+  </si>
+  <si>
+    <t>C321 C331</t>
+  </si>
+  <si>
+    <t>900410-13</t>
+  </si>
+  <si>
+    <t>4.7µF 16V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>TH 5mm</t>
+  </si>
+  <si>
+    <t>667-EEU-EB1H4R7SB</t>
+  </si>
+  <si>
+    <t>C913</t>
+  </si>
+  <si>
+    <t>390101-06</t>
+  </si>
+  <si>
+    <t>10µF 35V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>667-EEU-EB1J100SB</t>
+  </si>
+  <si>
+    <t>C306 C712</t>
+  </si>
+  <si>
+    <t>390101-04</t>
+  </si>
+  <si>
+    <t>22µF 35V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>C324 and C334 can be bipolar</t>
+  </si>
+  <si>
+    <t>667-EEU-FR1H220B</t>
+  </si>
+  <si>
+    <t>C303 C304 C324 C334</t>
+  </si>
+  <si>
+    <t>251894-50</t>
+  </si>
+  <si>
+    <t>47µF 35V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>667-EEU-FR1E470B</t>
+  </si>
+  <si>
+    <t>C821 C822</t>
+  </si>
+  <si>
+    <t>390101-02</t>
+  </si>
+  <si>
+    <t>100µF 16V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>667-EEU-FR1C101B</t>
+  </si>
+  <si>
+    <t>C811 C812 C813 C814 C815 C816</t>
+  </si>
+  <si>
+    <t>251894-18</t>
+  </si>
+  <si>
+    <t>1000µF 10V - Aluminum Electrolytic</t>
+  </si>
+  <si>
+    <t>height &lt; 24mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 667-EEU-FR1C102LB</t>
+  </si>
+  <si>
+    <t>C307 C401 C402</t>
+  </si>
+  <si>
+    <t>251029-06</t>
+  </si>
+  <si>
+    <t>Varicap 6.8pF – 45pF</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>901550-64</t>
+  </si>
+  <si>
+    <t>10Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-10R</t>
+  </si>
+  <si>
+    <t>R301 R302</t>
+  </si>
+  <si>
+    <t>901550-90</t>
+  </si>
+  <si>
+    <t>27Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-27R</t>
+  </si>
+  <si>
+    <t>R101 R102</t>
+  </si>
+  <si>
+    <t>901550-56</t>
+  </si>
+  <si>
+    <t>47Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-47R</t>
+  </si>
+  <si>
+    <t>R103 R104 R105 R106 R107 R113</t>
+  </si>
+  <si>
+    <t>901550-94</t>
+  </si>
+  <si>
+    <t>68Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-68R</t>
+  </si>
+  <si>
+    <t>E104 E105 FB101 R109 R111 R112 R114</t>
+  </si>
+  <si>
+    <t>901550-49</t>
+  </si>
+  <si>
+    <t>100Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-100R</t>
+  </si>
+  <si>
+    <t>R507</t>
+  </si>
+  <si>
+    <t>901550-89</t>
+  </si>
+  <si>
+    <t>150Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-150R</t>
+  </si>
+  <si>
+    <t>FB102 R409</t>
+  </si>
+  <si>
+    <t>901550-108</t>
+  </si>
+  <si>
+    <t>360Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-360R</t>
+  </si>
+  <si>
+    <t>R321 R331</t>
+  </si>
+  <si>
+    <t>901550-57</t>
+  </si>
+  <si>
+    <t>390Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-390R</t>
+  </si>
+  <si>
+    <t>R325 R335</t>
+  </si>
+  <si>
+    <t>901550-58</t>
+  </si>
+  <si>
+    <t>470Ω - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>Skip R913 on Rämixx500</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-470R</t>
+  </si>
+  <si>
+    <t>R911 R913</t>
+  </si>
+  <si>
+    <t>901550-01</t>
+  </si>
+  <si>
+    <t>1kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-1K</t>
+  </si>
+  <si>
+    <t>R191 R192 R303 R304 R305 R324 R334 R713 R915 R916</t>
+  </si>
+  <si>
+    <t>901550-23</t>
+  </si>
+  <si>
+    <t>2.7kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-2K7</t>
+  </si>
+  <si>
+    <t>R307 R502</t>
+  </si>
+  <si>
+    <t>901550-19</t>
+  </si>
+  <si>
+    <t>4.7kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-4K7</t>
+  </si>
+  <si>
+    <t>R201 R202 R402 R403 R404 R503 R504</t>
+  </si>
+  <si>
+    <t>901550-20</t>
+  </si>
+  <si>
+    <t>10kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-10K</t>
+  </si>
+  <si>
+    <t>R306 R308 R322 R323 R332 R333 R339 R501 R502 R506 R914</t>
+  </si>
+  <si>
+    <t>901550-22</t>
+  </si>
+  <si>
+    <t>47kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-47K</t>
+  </si>
+  <si>
+    <t>R712</t>
+  </si>
+  <si>
+    <t>901550-82</t>
+  </si>
+  <si>
+    <t>470kΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-470K</t>
+  </si>
+  <si>
+    <t>R326 R336</t>
+  </si>
+  <si>
+    <t>901550-84</t>
+  </si>
+  <si>
+    <t>1MΩ - 1/4W 5%</t>
+  </si>
+  <si>
+    <t>603-MF0207FTE52-1M</t>
+  </si>
+  <si>
+    <t>R711</t>
+  </si>
+  <si>
+    <t>901600-55</t>
+  </si>
+  <si>
+    <t>0.47Ω - 1/2W 5%</t>
+  </si>
+  <si>
+    <t>603-FMP100JR-52-0R47</t>
+  </si>
+  <si>
+    <t>R405</t>
+  </si>
+  <si>
+    <t>901600-36</t>
+  </si>
+  <si>
+    <t>10Ω - 1/2W 5%</t>
+  </si>
+  <si>
+    <t>603-FMP100JR-52-10R</t>
+  </si>
+  <si>
+    <t>R309</t>
+  </si>
+  <si>
+    <t>901600-50</t>
+  </si>
+  <si>
+    <t>4.7Ω - 1/2W 5%</t>
+  </si>
+  <si>
+    <t>or 5.1Ω</t>
+  </si>
+  <si>
+    <t>603-FMP100JR-52-4R7</t>
+  </si>
+  <si>
+    <t>R401 R406 R408</t>
+  </si>
+  <si>
+    <t>901600-15</t>
+  </si>
+  <si>
+    <t>47Ω - 1/2W 5%</t>
+  </si>
+  <si>
+    <t>603-FMP100JR-52-47R</t>
+  </si>
+  <si>
+    <t>E501 E502 E503</t>
+  </si>
+  <si>
+    <t>390227-08</t>
+  </si>
+  <si>
+    <t>39Ω Isolated Resistor Network, 5 Elements</t>
+  </si>
+  <si>
+    <t>or 22Ω</t>
+  </si>
+  <si>
+    <t>SIP10</t>
+  </si>
+  <si>
+    <t>652-4610X-2LF-39</t>
+  </si>
+  <si>
+    <t>RP103</t>
+  </si>
+  <si>
     <t>390227-06</t>
-  </si>
-  <si>
-    <t>74HCT245, Octal Tri-State Bus Transceiver</t>
-  </si>
-  <si>
-    <t>595-SN74HCT245N</t>
-  </si>
-  <si>
-    <t>U40 U41</t>
-  </si>
-  <si>
-    <t>901523-01</t>
-  </si>
-  <si>
-    <t>NE555, Timer</t>
-  </si>
-  <si>
-    <t>DIP8</t>
-  </si>
-  <si>
-    <t>595-NE555P</t>
-  </si>
-  <si>
-    <t>U42</t>
-  </si>
-  <si>
-    <t>Transistors</t>
-  </si>
-  <si>
-    <t>390254-01</t>
-  </si>
-  <si>
-    <t>MPF102 - N-Channel JFET</t>
-  </si>
-  <si>
-    <t>or PN4302. Rämixx500 SMD alternative: see below</t>
-  </si>
-  <si>
-    <t>TO-92</t>
-  </si>
-  <si>
-    <t>863-MPF102</t>
-  </si>
-  <si>
-    <t>Q321 Q331</t>
-  </si>
-  <si>
-    <t>902658-01</t>
-  </si>
-  <si>
-    <t>2N3904 - NPN</t>
-  </si>
-  <si>
-    <t>637-2N3904</t>
-  </si>
-  <si>
-    <t>Q501 Q711</t>
-  </si>
-  <si>
-    <t>902707-01</t>
-  </si>
-  <si>
-    <t>2N3906 - PNP</t>
-  </si>
-  <si>
-    <t>637-2N3906</t>
-  </si>
-  <si>
-    <t>Q301 Q502 Q503</t>
-  </si>
-  <si>
-    <t>Diodes</t>
-  </si>
-  <si>
-    <t>900850-01</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>or 1N914</t>
-  </si>
-  <si>
-    <t>TH</t>
-  </si>
-  <si>
-    <t>512-1N4148</t>
-  </si>
-  <si>
-    <t>D501 D911 D912</t>
-  </si>
-  <si>
-    <t>Capacitors</t>
-  </si>
-  <si>
-    <t>390082-01</t>
-  </si>
-  <si>
-    <t>10nF - MLC Z5U</t>
-  </si>
-  <si>
-    <t>Axial</t>
-  </si>
-  <si>
-    <t>80-C410C103M5R-TR</t>
-  </si>
-  <si>
-    <t>C7 C8 C10 C12 C15 C32 C33 C34 C35 C36 C37 C39 C308 C701 C713 C800 C801 C802 C803</t>
-  </si>
-  <si>
-    <t>390082-02</t>
-  </si>
-  <si>
-    <t>100nF - MLC Z5U</t>
-  </si>
-  <si>
-    <t>80-C412C104K5R-TR</t>
-  </si>
-  <si>
-    <t>C711</t>
-  </si>
-  <si>
-    <t>390082-04</t>
-  </si>
-  <si>
-    <t>330nF - MLC Z5U</t>
-  </si>
-  <si>
-    <t>80-C440C334K5R-TR</t>
-  </si>
-  <si>
-    <t>C1 C2 C3 C4 C5 C6 C9 C11 C13 C14 C16 C17 C18 C19 C20 C40 C41 C42 C301 C302 C305 C325 C335 C501 C502 C804</t>
-  </si>
-  <si>
-    <t>900462-21</t>
-  </si>
-  <si>
-    <t>22pF - MLC NP0</t>
-  </si>
-  <si>
-    <t>594-A220J15C0GH5TAA</t>
-  </si>
-  <si>
-    <t>C911 E666</t>
-  </si>
-  <si>
-    <t>900462-29</t>
-  </si>
-  <si>
-    <t>47pF - MLC NP0</t>
-  </si>
-  <si>
-    <t>594-A470J15C0GH5TAA</t>
-  </si>
-  <si>
-    <t>E102 E103 E106 E107 E108 E109 E791 E792 E793 E794</t>
-  </si>
-  <si>
-    <t>900463-16</t>
-  </si>
-  <si>
-    <t>1nF - MLC X7R</t>
-  </si>
-  <si>
-    <t>80-C420C102J1G-TR</t>
-  </si>
-  <si>
-    <t>C411 C412 C413 C421 C422 C423</t>
-  </si>
-  <si>
-    <t>900463-23</t>
-  </si>
-  <si>
-    <t>3.9nF - MLC X7R</t>
-  </si>
-  <si>
-    <t>80-C430C392GAG5TA</t>
-  </si>
-  <si>
-    <t>C323 C333</t>
-  </si>
-  <si>
-    <t>900463-26</t>
-  </si>
-  <si>
-    <t>6.8nF - MLC X7R</t>
-  </si>
-  <si>
-    <t>80-C430C682GAG5TA</t>
-  </si>
-  <si>
-    <t>C322 C332</t>
-  </si>
-  <si>
-    <t>900463-36</t>
-  </si>
-  <si>
-    <t>47nF - MLC X7R</t>
-  </si>
-  <si>
-    <t>80-C420C473J5G5TA</t>
-  </si>
-  <si>
-    <t>C311 C312 C313 C314</t>
-  </si>
-  <si>
-    <t>900463-37</t>
-  </si>
-  <si>
-    <t>0.1µF - MLC XR7</t>
-  </si>
-  <si>
-    <t>80-C430C104F3G5TA</t>
-  </si>
-  <si>
-    <t>C321 C331</t>
-  </si>
-  <si>
-    <t>900410-13</t>
-  </si>
-  <si>
-    <t>4.7µF 16V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>TH 5mm</t>
-  </si>
-  <si>
-    <t>667-EEU-EB1H4R7SB</t>
-  </si>
-  <si>
-    <t>C913</t>
-  </si>
-  <si>
-    <t>390101-06</t>
-  </si>
-  <si>
-    <t>10µF 35V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>667-EEU-EB1J100SB</t>
-  </si>
-  <si>
-    <t>C306 C712</t>
-  </si>
-  <si>
-    <t>390101-04</t>
-  </si>
-  <si>
-    <t>22µF 35V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>C324 and C334 can be bipolar</t>
-  </si>
-  <si>
-    <t>667-EEU-FR1H220B</t>
-  </si>
-  <si>
-    <t>C303 C304 C324 C334</t>
-  </si>
-  <si>
-    <t>251894-50</t>
-  </si>
-  <si>
-    <t>47µF 35V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>667-EEU-FR1E470B</t>
-  </si>
-  <si>
-    <t>C821 C822</t>
-  </si>
-  <si>
-    <t>390101-02</t>
-  </si>
-  <si>
-    <t>100µF 16V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>667-EEU-FR1C101B</t>
-  </si>
-  <si>
-    <t>C811 C812 C813 C814 C815 C816</t>
-  </si>
-  <si>
-    <t>251894-18</t>
-  </si>
-  <si>
-    <t>1000µF 10V - Aluminum Electrolytic</t>
-  </si>
-  <si>
-    <t>height &lt; 24mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 667-EEU-FR1C102LB</t>
-  </si>
-  <si>
-    <t>C307 C401 C402</t>
-  </si>
-  <si>
-    <t>251029-06</t>
-  </si>
-  <si>
-    <t>Varicap 6.8pF – 45pF</t>
-  </si>
-  <si>
-    <t>TC9</t>
-  </si>
-  <si>
-    <t>Resistors</t>
-  </si>
-  <si>
-    <t>901550-64</t>
-  </si>
-  <si>
-    <t>10Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-10R</t>
-  </si>
-  <si>
-    <t>R301 R302</t>
-  </si>
-  <si>
-    <t>901550-90</t>
-  </si>
-  <si>
-    <t>27Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-27R</t>
-  </si>
-  <si>
-    <t>R101 R102</t>
-  </si>
-  <si>
-    <t>901550-56</t>
-  </si>
-  <si>
-    <t>47Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-47R</t>
-  </si>
-  <si>
-    <t>R103 R104 R105 R106 R107 R113</t>
-  </si>
-  <si>
-    <t>901550-94</t>
-  </si>
-  <si>
-    <t>68Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-68R</t>
-  </si>
-  <si>
-    <t>E104 E105 FB101 R109 R111 R112 R114</t>
-  </si>
-  <si>
-    <t>901550-49</t>
-  </si>
-  <si>
-    <t>100Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-100R</t>
-  </si>
-  <si>
-    <t>R507</t>
-  </si>
-  <si>
-    <t>901550-89</t>
-  </si>
-  <si>
-    <t>150Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-150R</t>
-  </si>
-  <si>
-    <t>FB102 R409</t>
-  </si>
-  <si>
-    <t>901550-108</t>
-  </si>
-  <si>
-    <t>360Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-360R</t>
-  </si>
-  <si>
-    <t>R321 R331</t>
-  </si>
-  <si>
-    <t>901550-57</t>
-  </si>
-  <si>
-    <t>390Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-390R</t>
-  </si>
-  <si>
-    <t>R325 R335</t>
-  </si>
-  <si>
-    <t>901550-58</t>
-  </si>
-  <si>
-    <t>470Ω - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>Skip R913 on Rämixx500</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-470R</t>
-  </si>
-  <si>
-    <t>R911 R913</t>
-  </si>
-  <si>
-    <t>901550-01</t>
-  </si>
-  <si>
-    <t>1kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-1K</t>
-  </si>
-  <si>
-    <t>R191 R192 R303 R304 R305 R324 R334 R713 R915 R916</t>
-  </si>
-  <si>
-    <t>901550-23</t>
-  </si>
-  <si>
-    <t>2.7kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-2K7</t>
-  </si>
-  <si>
-    <t>R307 R502</t>
-  </si>
-  <si>
-    <t>901550-19</t>
-  </si>
-  <si>
-    <t>4.7kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-4K7</t>
-  </si>
-  <si>
-    <t>R201 R202 R402 R403 R404 R503 R504</t>
-  </si>
-  <si>
-    <t>901550-20</t>
-  </si>
-  <si>
-    <t>10kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-10K</t>
-  </si>
-  <si>
-    <t>R306 R308 R322 R323 R332 R333 R339 R501 R502 R506 R914</t>
-  </si>
-  <si>
-    <t>901550-22</t>
-  </si>
-  <si>
-    <t>47kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-47K</t>
-  </si>
-  <si>
-    <t>R712</t>
-  </si>
-  <si>
-    <t>901550-82</t>
-  </si>
-  <si>
-    <t>470kΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-470K</t>
-  </si>
-  <si>
-    <t>R326 R336</t>
-  </si>
-  <si>
-    <t>901550-84</t>
-  </si>
-  <si>
-    <t>1MΩ - 1/4W 5%</t>
-  </si>
-  <si>
-    <t>603-MF0207FTE52-1M</t>
-  </si>
-  <si>
-    <t>R711</t>
-  </si>
-  <si>
-    <t>901600-55</t>
-  </si>
-  <si>
-    <t>0.47Ω - 1/2W 5%</t>
-  </si>
-  <si>
-    <t>603-FMP100JR-52-0R47</t>
-  </si>
-  <si>
-    <t>R405</t>
-  </si>
-  <si>
-    <t>901600-36</t>
-  </si>
-  <si>
-    <t>10Ω - 1/2W 5%</t>
-  </si>
-  <si>
-    <t>603-FMP100JR-52-10R</t>
-  </si>
-  <si>
-    <t>R309</t>
-  </si>
-  <si>
-    <t>901600-50</t>
-  </si>
-  <si>
-    <t>4.7Ω - 1/2W 5%</t>
-  </si>
-  <si>
-    <t>or 5.1Ω</t>
-  </si>
-  <si>
-    <t>603-FMP100JR-52-4R7</t>
-  </si>
-  <si>
-    <t>R401 R406 R408</t>
-  </si>
-  <si>
-    <t>901600-15</t>
-  </si>
-  <si>
-    <t>47Ω - 1/2W 5%</t>
-  </si>
-  <si>
-    <t>603-FMP100JR-52-47R</t>
-  </si>
-  <si>
-    <t>E501 E502 E503</t>
-  </si>
-  <si>
-    <t>390227-08</t>
-  </si>
-  <si>
-    <t>39Ω Isolated Resistor Network, 5 Elements</t>
-  </si>
-  <si>
-    <t>or 22Ω</t>
-  </si>
-  <si>
-    <t>SIP10</t>
-  </si>
-  <si>
-    <t>652-4610X-2LF-39</t>
-  </si>
-  <si>
-    <t>RP103</t>
   </si>
   <si>
     <t>47Ω Isolated Resistor Network, 5 Elements</t>
@@ -1667,7 +1670,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Version: 0.5 (2024-04-16)
+      <t xml:space="preserve">Version: 0.6 (2024-04-28)
 </t>
     </r>
     <r>
@@ -3598,107 +3601,107 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>297</v>
       </c>
       <c r="B77">
         <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E77" t="s">
         <v>294</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B78">
         <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E78" t="s">
         <v>294</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E79" t="s">
         <v>294</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B80">
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E80" t="s">
         <v>294</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E81" t="s">
         <v>294</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3709,205 +3712,205 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B83">
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D83" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E83" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B84">
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D84" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E84" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B85">
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D85" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E85" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B86">
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D86" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E86" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B87">
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D87" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E87" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B88">
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D88" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E88" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D89" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E89" t="s">
         <v>133</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B90">
         <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E90" t="s">
         <v>133</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E91" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3918,67 +3921,67 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D93" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E93" t="s">
         <v>61</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D94" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E94" t="s">
         <v>61</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
       <c r="C95" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E95" t="s">
         <v>133</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3989,285 +3992,285 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B97">
         <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D97" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E97" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D98" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B99">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D99" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B100">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D100" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E100" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D101" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E101" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B102">
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D102" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E102" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D103" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B104">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D104" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E104" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B105">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D105" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D106" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E106" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D107" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E107" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D108" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E108" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D109" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E109" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4278,41 +4281,41 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D111" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D112" t="s">
         <v>23</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4323,22 +4326,22 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B114">
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D114" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E114" t="s">
         <v>34</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>35</v>
@@ -4346,22 +4349,22 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
       <c r="C115" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D115" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E115" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>44</v>
@@ -4369,45 +4372,45 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B116">
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D116" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E116" t="s">
         <v>24</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
       <c r="C117" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D117" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E117" t="s">
         <v>39</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>40</v>
@@ -4415,22 +4418,22 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B118">
         <v>1</v>
       </c>
       <c r="C118" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D118" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E118" t="s">
         <v>17</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>18</v>
@@ -4438,7 +4441,7 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4452,13 +4455,13 @@
         <v>1</v>
       </c>
       <c r="C120" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E120" t="s">
         <v>111</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>113</v>
@@ -4469,16 +4472,16 @@
         <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E121" t="s">
         <v>61</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -4486,16 +4489,16 @@
         <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E122" t="s">
         <v>66</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -4503,13 +4506,13 @@
         <v>1</v>
       </c>
       <c r="C123" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E123" t="s">
         <v>48</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>49</v>
@@ -4517,22 +4520,22 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B124">
         <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E124" t="s">
         <v>52</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -4540,13 +4543,13 @@
         <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E125" t="s">
         <v>52</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>71</v>
@@ -4554,25 +4557,25 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B126">
         <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D126" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E126" t="s">
         <v>294</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -4580,21 +4583,21 @@
         <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D127" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E127" t="s">
         <v>180</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4608,19 +4611,19 @@
         <v>4</v>
       </c>
       <c r="C129" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D129" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E129" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -4628,19 +4631,19 @@
         <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D130" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E130" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -4648,19 +4651,19 @@
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D131" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E131" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -4674,7 +4677,7 @@
         <v>131</v>
       </c>
       <c r="D132" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E132" t="s">
         <v>133</v>
@@ -4683,7 +4686,7 @@
         <v>134</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -4697,7 +4700,7 @@
         <v>126</v>
       </c>
       <c r="D133" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E133" t="s">
         <v>118</v>
@@ -4706,7 +4709,7 @@
         <v>127</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -4720,7 +4723,7 @@
         <v>259</v>
       </c>
       <c r="D134" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E134" t="s">
         <v>133</v>
@@ -4729,7 +4732,7 @@
         <v>260</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -4743,7 +4746,7 @@
         <v>263</v>
       </c>
       <c r="D135" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E135" t="s">
         <v>133</v>
@@ -4752,7 +4755,7 @@
         <v>264</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4766,7 +4769,7 @@
         <v>143</v>
       </c>
       <c r="D136" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E136" t="s">
         <v>139</v>
@@ -4775,7 +4778,7 @@
         <v>144</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -4783,19 +4786,19 @@
         <v>1</v>
       </c>
       <c r="C137" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D137" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E137" t="s">
         <v>133</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4803,16 +4806,16 @@
         <v>1</v>
       </c>
       <c r="C138" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E138" t="s">
         <v>133</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -4820,16 +4823,16 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D139" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -4837,16 +4840,16 @@
         <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D140" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4854,36 +4857,36 @@
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D141" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B142">
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D142" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E142" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4891,21 +4894,21 @@
         <v>1</v>
       </c>
       <c r="C143" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D143" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="60" customHeight="1">
       <c r="A145" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>